<commit_message>
Acertos de última hora
</commit_message>
<xml_diff>
--- a/enderecos.xlsx
+++ b/enderecos.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Origem" sheetId="1" r:id="rId1"/>
@@ -16,23 +16,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
-  <si>
-    <t>Rua São Francisco Xavier, 374 A, Maracana, Rio de Janeiro</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>Endereco</t>
   </si>
   <si>
-    <t>Rua Nicarágua, 294, penha, Rio de janeiro</t>
-  </si>
-  <si>
-    <t>Rua Haddock Lobo, 5, Estacio, Rio de Janeiro</t>
-  </si>
-  <si>
-    <t>Rua Barão de Mesquita, 972, Verdun, Rio de Janeiro</t>
-  </si>
-  <si>
     <t>Rua Barão do Bom Retiro, 1.115, Engenho novo, Rio de Janeiro</t>
   </si>
   <si>
@@ -43,6 +31,27 @@
   </si>
   <si>
     <t>TempoMaximoDeEntregaEmHoras</t>
+  </si>
+  <si>
+    <t>Rua Uruguai, 471, Rio de Janeiro - RJ</t>
+  </si>
+  <si>
+    <t>Rua Barão de Mesquita, 622-628 - Tijuca Rio de Janeiro - RJ, 20540-001</t>
+  </si>
+  <si>
+    <t>Rua Uruguai, 128-162 - Andaraí Rio de Janeiro - RJ, 20510-060</t>
+  </si>
+  <si>
+    <t>Rua Gomes Braga, 50 - Andaraí Rio de Janeiro - RJ</t>
+  </si>
+  <si>
+    <t>Av. Mal. Rondon, 1853 - Riachuelo Rio de Janeiro - RJ, 20950-006</t>
+  </si>
+  <si>
+    <t>Rua Visc. de Santa Isabel, 592 - Grajaú Rio de Janeiro - RJ 20560-121</t>
+  </si>
+  <si>
+    <t>Rua Barão do Bom Retiro, 1199 - Engenho Novo Rio de Janeiro - RJ, 20715-004</t>
   </si>
 </sst>
 </file>
@@ -384,7 +393,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -394,12 +403,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -410,10 +419,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -423,27 +432,42 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -456,7 +480,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
@@ -468,15 +492,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B2">
         <v>1</v>

</xml_diff>